<commit_message>
trying to get file path stuff worked out
</commit_message>
<xml_diff>
--- a/Data/timings_both_models_8-8_treatments.xlsx
+++ b/Data/timings_both_models_8-8_treatments.xlsx
@@ -541,25 +541,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2.12</v>
+        <v>2.088</v>
       </c>
       <c r="G2">
         <v>0.042</v>
       </c>
       <c r="H2">
-        <v>1.209</v>
+        <v>1.27</v>
       </c>
       <c r="I2">
-        <v>0.383</v>
+        <v>0.376</v>
       </c>
       <c r="J2">
-        <v>0.456</v>
+        <v>0.369</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.00019</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -579,25 +579,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>2.144</v>
+        <v>2.053</v>
       </c>
       <c r="G3">
-        <v>0.045</v>
+        <v>0.051</v>
       </c>
       <c r="H3">
-        <v>1.206</v>
+        <v>1.117</v>
       </c>
       <c r="I3">
-        <v>0.46</v>
+        <v>0.369</v>
       </c>
       <c r="J3">
-        <v>0.402</v>
+        <v>0.434</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.0002</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -617,25 +617,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>2.203</v>
+        <v>2.023</v>
       </c>
       <c r="G4">
-        <v>0.045</v>
+        <v>0.041</v>
       </c>
       <c r="H4">
-        <v>1.245</v>
+        <v>1.131</v>
       </c>
       <c r="I4">
-        <v>0.466</v>
+        <v>0.44</v>
       </c>
       <c r="J4">
-        <v>0.418</v>
+        <v>0.381</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00021</v>
+        <v>0.00019</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -655,25 +655,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>2.246</v>
+        <v>2.058</v>
       </c>
       <c r="G5">
-        <v>0.046</v>
+        <v>0.043</v>
       </c>
       <c r="H5">
-        <v>1.328</v>
+        <v>1.217</v>
       </c>
       <c r="I5">
-        <v>0.419</v>
+        <v>0.378</v>
       </c>
       <c r="J5">
-        <v>0.422</v>
+        <v>0.39</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.00021</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -693,25 +693,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>2.327</v>
+        <v>2.178</v>
       </c>
       <c r="G6">
-        <v>0.052</v>
+        <v>0.043</v>
       </c>
       <c r="H6">
-        <v>1.276</v>
+        <v>1.253</v>
       </c>
       <c r="I6">
-        <v>0.431</v>
+        <v>0.398</v>
       </c>
       <c r="J6">
-        <v>0.485</v>
+        <v>0.455</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.00021</v>
+        <v>0.0002</v>
       </c>
     </row>
   </sheetData>
@@ -1053,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>3.307</v>
+        <v>3.114</v>
       </c>
       <c r="G2">
         <v>0.002</v>
@@ -1062,16 +1062,16 @@
         <v>0.004</v>
       </c>
       <c r="I2">
-        <v>1.217</v>
+        <v>1.097</v>
       </c>
       <c r="J2">
-        <v>1.222</v>
+        <v>1.225</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.00023</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1091,25 +1091,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>3.233</v>
+        <v>3.191</v>
       </c>
       <c r="G3">
         <v>0.002</v>
       </c>
       <c r="H3">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="I3">
-        <v>1.204</v>
+        <v>1.235</v>
       </c>
       <c r="J3">
-        <v>1.274</v>
+        <v>1.216</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.00024</v>
+        <v>0.00023</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1129,7 +1129,7 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>3.252</v>
+        <v>3.118</v>
       </c>
       <c r="G4">
         <v>0.002</v>
@@ -1138,16 +1138,16 @@
         <v>0.005</v>
       </c>
       <c r="I4">
-        <v>1.234</v>
+        <v>1.181</v>
       </c>
       <c r="J4">
-        <v>1.231</v>
+        <v>1.207</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00023</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1167,25 +1167,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>3.203</v>
+        <v>3.165</v>
       </c>
       <c r="G5">
         <v>0.002</v>
       </c>
       <c r="H5">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="I5">
-        <v>1.224</v>
+        <v>1.212</v>
       </c>
       <c r="J5">
-        <v>1.212</v>
+        <v>1.219</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.00023</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1205,19 +1205,19 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>3.186</v>
+        <v>3.233</v>
       </c>
       <c r="G6">
         <v>0.002</v>
       </c>
       <c r="H6">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="I6">
-        <v>1.221</v>
+        <v>1.254</v>
       </c>
       <c r="J6">
-        <v>1.217</v>
+        <v>1.247</v>
       </c>
       <c r="K6">
         <v>1000</v>
@@ -1565,25 +1565,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2.12</v>
+        <v>2.088</v>
       </c>
       <c r="G2">
         <v>0.042</v>
       </c>
       <c r="H2">
-        <v>1.209</v>
+        <v>1.27</v>
       </c>
       <c r="I2">
-        <v>0.383</v>
+        <v>0.376</v>
       </c>
       <c r="J2">
-        <v>0.456</v>
+        <v>0.369</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.00019</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1603,25 +1603,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>2.144</v>
+        <v>2.053</v>
       </c>
       <c r="G3">
-        <v>0.045</v>
+        <v>0.051</v>
       </c>
       <c r="H3">
-        <v>1.206</v>
+        <v>1.117</v>
       </c>
       <c r="I3">
-        <v>0.46</v>
+        <v>0.369</v>
       </c>
       <c r="J3">
-        <v>0.402</v>
+        <v>0.434</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.0002</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1641,25 +1641,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>2.203</v>
+        <v>2.023</v>
       </c>
       <c r="G4">
-        <v>0.045</v>
+        <v>0.041</v>
       </c>
       <c r="H4">
-        <v>1.245</v>
+        <v>1.131</v>
       </c>
       <c r="I4">
-        <v>0.466</v>
+        <v>0.44</v>
       </c>
       <c r="J4">
-        <v>0.418</v>
+        <v>0.381</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00021</v>
+        <v>0.00019</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1679,25 +1679,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>2.246</v>
+        <v>2.058</v>
       </c>
       <c r="G5">
-        <v>0.046</v>
+        <v>0.043</v>
       </c>
       <c r="H5">
-        <v>1.328</v>
+        <v>1.217</v>
       </c>
       <c r="I5">
-        <v>0.419</v>
+        <v>0.378</v>
       </c>
       <c r="J5">
-        <v>0.422</v>
+        <v>0.39</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.00021</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1717,25 +1717,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>2.327</v>
+        <v>2.178</v>
       </c>
       <c r="G6">
-        <v>0.052</v>
+        <v>0.043</v>
       </c>
       <c r="H6">
-        <v>1.276</v>
+        <v>1.253</v>
       </c>
       <c r="I6">
-        <v>0.431</v>
+        <v>0.398</v>
       </c>
       <c r="J6">
-        <v>0.485</v>
+        <v>0.455</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.00021</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1755,7 +1755,7 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>3.307</v>
+        <v>3.114</v>
       </c>
       <c r="G7">
         <v>0.002</v>
@@ -1764,16 +1764,16 @@
         <v>0.004</v>
       </c>
       <c r="I7">
-        <v>1.217</v>
+        <v>1.097</v>
       </c>
       <c r="J7">
-        <v>1.222</v>
+        <v>1.225</v>
       </c>
       <c r="K7">
         <v>1000</v>
       </c>
       <c r="L7">
-        <v>0.00023</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1793,25 +1793,25 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>3.233</v>
+        <v>3.191</v>
       </c>
       <c r="G8">
         <v>0.002</v>
       </c>
       <c r="H8">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="I8">
-        <v>1.204</v>
+        <v>1.235</v>
       </c>
       <c r="J8">
-        <v>1.274</v>
+        <v>1.216</v>
       </c>
       <c r="K8">
         <v>1000</v>
       </c>
       <c r="L8">
-        <v>0.00024</v>
+        <v>0.00023</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1831,7 +1831,7 @@
         <v>3</v>
       </c>
       <c r="F9">
-        <v>3.252</v>
+        <v>3.118</v>
       </c>
       <c r="G9">
         <v>0.002</v>
@@ -1840,16 +1840,16 @@
         <v>0.005</v>
       </c>
       <c r="I9">
-        <v>1.234</v>
+        <v>1.181</v>
       </c>
       <c r="J9">
-        <v>1.231</v>
+        <v>1.207</v>
       </c>
       <c r="K9">
         <v>1000</v>
       </c>
       <c r="L9">
-        <v>0.00023</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1869,25 +1869,25 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>3.203</v>
+        <v>3.165</v>
       </c>
       <c r="G10">
         <v>0.002</v>
       </c>
       <c r="H10">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="I10">
-        <v>1.224</v>
+        <v>1.212</v>
       </c>
       <c r="J10">
-        <v>1.212</v>
+        <v>1.219</v>
       </c>
       <c r="K10">
         <v>1000</v>
       </c>
       <c r="L10">
-        <v>0.00023</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1907,19 +1907,19 @@
         <v>5</v>
       </c>
       <c r="F11">
-        <v>3.186</v>
+        <v>3.233</v>
       </c>
       <c r="G11">
         <v>0.002</v>
       </c>
       <c r="H11">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="I11">
-        <v>1.221</v>
+        <v>1.254</v>
       </c>
       <c r="J11">
-        <v>1.217</v>
+        <v>1.247</v>
       </c>
       <c r="K11">
         <v>1000</v>

</xml_diff>